<commit_message>
recoding of bistline data
</commit_message>
<xml_diff>
--- a/data-extra/ira_comparison_raw/VariableMapping.xlsx
+++ b/data-extra/ira_comparison_raw/VariableMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-extra\ira_comparison_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9ED90B-CE4C-41C6-BFBC-D79134BCBEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972CFA79-8BBB-4A1D-86ED-90CD0F042368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA92EE2D-36A0-48E9-BFBF-9573E46ECB63}"/>
   </bookViews>
@@ -219,21 +219,12 @@
     <t>Fossil Consumption - Coal</t>
   </si>
   <si>
-    <t>Final Energy|Coal</t>
-  </si>
-  <si>
     <t>Fossil Consumption - Natural Gas</t>
   </si>
   <si>
-    <t>Final Energy|Gas</t>
-  </si>
-  <si>
     <t>Fossil Consumption - Petroleum</t>
   </si>
   <si>
-    <t>Final Energy|Oil</t>
-  </si>
-  <si>
     <t>Non-CO2 GHG</t>
   </si>
   <si>
@@ -262,6 +253,15 @@
   </si>
   <si>
     <t>sum of Electricity Demand - Light-Duty Vehicles and -Other Transport</t>
+  </si>
+  <si>
+    <t>Primary Energy|Coal</t>
+  </si>
+  <si>
+    <t>Primary Energy|Gas</t>
+  </si>
+  <si>
+    <t>Primary Energy|Oil</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA515E4B-9157-4310-B5F6-E3E96B70C107}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,13 +926,13 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,36 +940,36 @@
         <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
         <v>33</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
         <v>33</v>
@@ -985,13 +985,13 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1001,6 +1001,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
@@ -1042,21 +1051,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B8B916ED2FB6A47AFA4E05A3E606BD3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a94e0fd8b44729910807c0515ebac9ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="3d00cabe-74f9-499f-ba26-1e0076cbc6cc" xmlns:ns6="2755580c-7c5f-43cf-bd85-5c868b718937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c46c8e9e737c7513e9b5f82e7b81653" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1477,7 +1472,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCCD16A-B1D9-494E-A9ED-75C0C6A6F828}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{490D51B6-E972-495C-9AF2-62BB75061D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1498,23 +1506,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCCD16A-B1D9-494E-A9ED-75C0C6A6F828}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC71AF99-F4A7-437B-87FB-091C0D1F1382}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303F5059-C929-45FC-82ED-C8A8B8964CF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1535,4 +1527,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC71AF99-F4A7-437B-87FB-091C0D1F1382}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
economy-wide co2 emissions added
</commit_message>
<xml_diff>
--- a/data-extra/ira_comparison_raw/VariableMapping.xlsx
+++ b/data-extra/ira_comparison_raw/VariableMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-extra\ira_comparison_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9018F9F-9698-4589-B336-C0D374A70077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD45EAD-1EEB-4755-B69B-24F0BEFACA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA92EE2D-36A0-48E9-BFBF-9573E46ECB63}"/>
+    <workbookView minimized="1" xWindow="1845" yWindow="1830" windowWidth="17250" windowHeight="8865" xr2:uid="{DA92EE2D-36A0-48E9-BFBF-9573E46ECB63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -625,18 +625,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA515E4B-9157-4310-B5F6-E3E96B70C107}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -655,7 +655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -663,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -674,7 +674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -682,7 +682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -693,7 +693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -704,7 +704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -712,7 +712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -720,7 +720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -728,7 +728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -736,7 +736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -744,7 +744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -752,7 +752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -760,7 +760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -768,7 +768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -776,7 +776,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -787,7 +787,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -795,7 +795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
@@ -803,7 +803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -811,7 +811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -822,7 +822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -833,7 +833,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -841,7 +841,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -849,7 +849,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -857,7 +857,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -865,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -873,7 +873,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -881,7 +881,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -889,7 +889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -897,7 +897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -905,7 +905,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -913,7 +913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -921,7 +921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -929,7 +929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -937,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -945,7 +945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -953,7 +953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -961,7 +961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -969,7 +969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -980,7 +980,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
@@ -988,7 +988,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -996,7 +996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
@@ -1058,20 +1058,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B8B916ED2FB6A47AFA4E05A3E606BD3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a94e0fd8b44729910807c0515ebac9ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="3d00cabe-74f9-499f-ba26-1e0076cbc6cc" xmlns:ns6="2755580c-7c5f-43cf-bd85-5c868b718937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c46c8e9e737c7513e9b5f82e7b81653" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1492,6 +1478,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{490D51B6-E972-495C-9AF2-62BB75061D28}">
   <ds:schemaRefs>
@@ -1514,22 +1514,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCCD16A-B1D9-494E-A9ED-75C0C6A6F828}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC71AF99-F4A7-437B-87FB-091C0D1F1382}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303F5059-C929-45FC-82ED-C8A8B8964CF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1550,4 +1534,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC71AF99-F4A7-437B-87FB-091C0D1F1382}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCCD16A-B1D9-494E-A9ED-75C0C6A6F828}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>